<commit_message>
various changes for conflator package
</commit_message>
<xml_diff>
--- a/model_network/npmrds_conflation/Conflation Testing.xlsx
+++ b/model_network/npmrds_conflation/Conflation Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\SACSIM19\model_network\npmrds_conflation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A58254B-5967-460A-AD43-5A88428E1ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A92E53-17B5-4DE1-BB2E-15311E2E2576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,15 +943,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -966,7 +966,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4143375" y="3333751"/>
+          <a:off x="3667125" y="352426"/>
           <a:ext cx="2095499" cy="962024"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1969,15 +1969,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1994,9 +1994,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="4352925" y="4810125"/>
-          <a:ext cx="1352551" cy="323850"/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2624137" y="3405188"/>
+          <a:ext cx="4333876" cy="152400"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -2026,16 +2026,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>390526</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2053,8 +2053,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="6362700" y="3124200"/>
-          <a:ext cx="1390651" cy="3733800"/>
+          <a:off x="4633912" y="1395413"/>
+          <a:ext cx="4371976" cy="4210050"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -3253,15 +3253,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>252413</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3279,13 +3279,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1" flipV="1">
-          <a:off x="4143375" y="3814763"/>
-          <a:ext cx="4033838" cy="6376988"/>
+          <a:off x="3667125" y="833437"/>
+          <a:ext cx="4510088" cy="9358313"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -98937"/>
-            <a:gd name="adj2" fmla="val 92606"/>
+            <a:gd name="adj1" fmla="val -5069"/>
+            <a:gd name="adj2" fmla="val 52570"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -6612,7 +6612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A433324D-ED3A-45BE-95FC-6A4BCCA59E80}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="S49" sqref="S49"/>
     </sheetView>
   </sheetViews>

</xml_diff>